<commit_message>
TEX: Add softmax and pooling appendix. Fix SFU table
</commit_message>
<xml_diff>
--- a/DOC/FLOP_Calculations.xlsx
+++ b/DOC/FLOP_Calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-6960" yWindow="-18580" windowWidth="48460" windowHeight="17640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="47100" windowHeight="22420" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CNN" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="64">
   <si>
     <t>X</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>% fanin</t>
+  </si>
+  <si>
+    <t>Weight for DNN</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -687,6 +689,9 @@
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -706,9 +711,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1186,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:Y42"/>
   <sheetViews>
-    <sheetView topLeftCell="M3" workbookViewId="0">
-      <selection activeCell="X40" sqref="X40"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="Y38" sqref="Y38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1202,12 +1204,12 @@
       <c r="O4" s="1">
         <v>32</v>
       </c>
-      <c r="Q4" s="33" t="s">
+      <c r="Q4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="34"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="36"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="37"/>
       <c r="U4" s="3"/>
     </row>
     <row r="5" spans="4:25" ht="30">
@@ -2408,7 +2410,7 @@
   <dimension ref="D4:AJ42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X28" sqref="X28"/>
+      <selection activeCell="Z37" sqref="Z37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2419,7 +2421,7 @@
     <col min="19" max="19" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.6640625" style="1" customWidth="1"/>
     <col min="21" max="23" width="10.83203125" style="1"/>
-    <col min="24" max="24" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="10.83203125" style="1"/>
     <col min="27" max="27" width="11.83203125" style="28" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.83203125" style="1"/>
@@ -2429,11 +2431,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:36">
-      <c r="M4" s="37" t="s">
+      <c r="M4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="38"/>
-      <c r="O4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="40"/>
       <c r="P4" s="3"/>
       <c r="V4" s="1" t="s">
         <v>51</v>
@@ -2481,6 +2483,9 @@
       </c>
       <c r="S5" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>50</v>
@@ -2612,7 +2617,7 @@
         <f>I8*J8*G6</f>
         <v>363</v>
       </c>
-      <c r="X8" s="1">
+      <c r="X8" s="15">
         <f>L8*W8</f>
         <v>105415200</v>
       </c>
@@ -2631,7 +2636,7 @@
       <c r="AB8" s="1">
         <v>25</v>
       </c>
-      <c r="AC8" s="40">
+      <c r="AC8" s="33">
         <f>L8/$L$28</f>
         <v>0.37590091955927429</v>
       </c>
@@ -2797,7 +2802,7 @@
         <f>I12*J12*G10</f>
         <v>2400</v>
       </c>
-      <c r="X12" s="1">
+      <c r="X12" s="15">
         <f>L12*W12</f>
         <v>447897600</v>
       </c>
@@ -2816,7 +2821,7 @@
       <c r="AB12" s="1">
         <v>30</v>
       </c>
-      <c r="AC12" s="40">
+      <c r="AC12" s="33">
         <f>L12/$L$28</f>
         <v>0.24157070665230718</v>
       </c>
@@ -2985,7 +2990,7 @@
         <f>I16*J16*G14</f>
         <v>2304</v>
       </c>
-      <c r="X16" s="1">
+      <c r="X16" s="15">
         <f>L16*W16</f>
         <v>149520384</v>
       </c>
@@ -3004,7 +3009,7 @@
       <c r="AB16" s="1">
         <v>30</v>
       </c>
-      <c r="AC16" s="40">
+      <c r="AC16" s="33">
         <f>L16/$L$28</f>
         <v>8.4002982354403122E-2</v>
       </c>
@@ -3089,7 +3094,7 @@
         <f>I18*J18*G16</f>
         <v>3456</v>
       </c>
-      <c r="X18" s="1">
+      <c r="X18" s="15">
         <f>L18*W18</f>
         <v>224280576</v>
       </c>
@@ -3108,7 +3113,7 @@
       <c r="AB18" s="1">
         <v>30</v>
       </c>
-      <c r="AC18" s="40">
+      <c r="AC18" s="33">
         <f>L18/$L$28</f>
         <v>8.4002982354403122E-2</v>
       </c>
@@ -3193,7 +3198,7 @@
         <f>I20*J20*G18</f>
         <v>3456</v>
       </c>
-      <c r="X20" s="1">
+      <c r="X20" s="15">
         <f>L20*W20</f>
         <v>149520384</v>
       </c>
@@ -3212,7 +3217,7 @@
       <c r="AB20" s="1">
         <v>30</v>
       </c>
-      <c r="AC20" s="40">
+      <c r="AC20" s="33">
         <f>L20/$L$28</f>
         <v>5.6001988236268743E-2</v>
       </c>
@@ -3293,7 +3298,7 @@
         <f>I22*J22*G20</f>
         <v>43264</v>
       </c>
-      <c r="X22" s="1">
+      <c r="X22" s="15">
         <f>L22*W22</f>
         <v>177209344</v>
       </c>
@@ -3312,7 +3317,7 @@
       <c r="AB22" s="1">
         <v>31</v>
       </c>
-      <c r="AC22" s="40">
+      <c r="AC22" s="33">
         <f>L22/$L$28</f>
         <v>5.3019633833153836E-3</v>
       </c>
@@ -3393,7 +3398,7 @@
         <f>G22</f>
         <v>4096</v>
       </c>
-      <c r="X24" s="1">
+      <c r="X24" s="15">
         <f>L24*W24</f>
         <v>16777216</v>
       </c>
@@ -3412,7 +3417,7 @@
       <c r="AB24" s="1">
         <v>31</v>
       </c>
-      <c r="AC24" s="40">
+      <c r="AC24" s="33">
         <f>L24/$L$28</f>
         <v>5.3019633833153836E-3</v>
       </c>
@@ -3496,7 +3501,7 @@
         <f>G24</f>
         <v>4096</v>
       </c>
-      <c r="X26" s="1">
+      <c r="X26" s="15">
         <f>L26*W26</f>
         <v>4194304</v>
       </c>
@@ -3515,7 +3520,7 @@
       <c r="AB26" s="1">
         <v>30</v>
       </c>
-      <c r="AC26" s="40">
+      <c r="AC26" s="33">
         <f>L26/$L$28</f>
         <v>1.3254908458288459E-3</v>
       </c>
@@ -3527,7 +3532,7 @@
       <c r="Q27" s="15"/>
       <c r="R27" s="15"/>
       <c r="S27" s="15"/>
-      <c r="X27" s="1">
+      <c r="X27" s="15">
         <f>SUM(X8:X26)</f>
         <v>1274815008</v>
       </c>
@@ -3566,7 +3571,7 @@
       <c r="W28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="X28" s="1">
+      <c r="X28" s="15">
         <f>X27/SUM(L8:L26)</f>
         <v>1650.151975809792</v>
       </c>
@@ -3712,11 +3717,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:19">
-      <c r="M4" s="37" t="s">
+      <c r="M4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="38"/>
-      <c r="O4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="40"/>
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="4:19" ht="30">

</xml_diff>

<commit_message>
TEX:Add reference to state-of-the-art in the results section
</commit_message>
<xml_diff>
--- a/DOC/FLOP_Calculations.xlsx
+++ b/DOC/FLOP_Calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="47100" windowHeight="22420" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CNN" sheetId="2" r:id="rId1"/>
@@ -12,6 +12,9 @@
     <sheet name="CNN tmp" sheetId="3" r:id="rId3"/>
     <sheet name="XU" sheetId="4" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="72">
   <si>
     <t>X</t>
   </si>
@@ -214,6 +217,30 @@
   </si>
   <si>
     <t>Weight for DNN</t>
+  </si>
+  <si>
+    <t>% operations</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>CONV-300</t>
+  </si>
+  <si>
+    <t>CONV-1000</t>
+  </si>
+  <si>
+    <t>FC-7</t>
+  </si>
+  <si>
+    <t>CONV2</t>
+  </si>
+  <si>
+    <t>CONV-294</t>
+  </si>
+  <si>
+    <t>Expected Bandwidth</t>
   </si>
 </sst>
 </file>
@@ -450,7 +477,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="143">
+  <cellStyleXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -594,8 +621,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -692,6 +741,9 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -714,7 +766,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="143">
+  <cellStyles count="165">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -786,6 +838,17 @@
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -857,11 +920,168 @@
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="PE"/>
+      <sheetName val="Manager"/>
+      <sheetName val="DRAM"/>
+      <sheetName val="Summary"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>CONV2</v>
+          </cell>
+          <cell r="B16">
+            <v>0.65</v>
+          </cell>
+          <cell r="C16">
+            <v>21.9648</v>
+          </cell>
+          <cell r="D16">
+            <v>59.63776</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>CONV-294</v>
+          </cell>
+          <cell r="B17">
+            <v>0.67</v>
+          </cell>
+          <cell r="C17">
+            <v>22.640640000000001</v>
+          </cell>
+          <cell r="D17">
+            <v>61.472768000000002</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>CONV-300</v>
+          </cell>
+          <cell r="B18">
+            <v>0.73</v>
+          </cell>
+          <cell r="C18">
+            <v>24.66816</v>
+          </cell>
+          <cell r="D18">
+            <v>66.977791999999994</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>FC-350</v>
+          </cell>
+          <cell r="B19">
+            <v>0.78</v>
+          </cell>
+          <cell r="C19">
+            <v>26.357760000000003</v>
+          </cell>
+          <cell r="D19">
+            <v>71.565312000000006</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>FC-500</v>
+          </cell>
+          <cell r="B20">
+            <v>0.84</v>
+          </cell>
+          <cell r="C20">
+            <v>28.385280000000002</v>
+          </cell>
+          <cell r="D20">
+            <v>77.070335999999998</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>FC-7</v>
+          </cell>
+          <cell r="B21">
+            <v>0.94</v>
+          </cell>
+          <cell r="C21">
+            <v>31.764479999999999</v>
+          </cell>
+          <cell r="D21">
+            <v>86.245375999999993</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>CONV-500</v>
+          </cell>
+          <cell r="B22">
+            <v>0.82</v>
+          </cell>
+          <cell r="C22">
+            <v>27.709440000000001</v>
+          </cell>
+          <cell r="D22">
+            <v>75.235327999999996</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>CONV-1000</v>
+          </cell>
+          <cell r="B23">
+            <v>0.89</v>
+          </cell>
+          <cell r="C23">
+            <v>30.07488</v>
+          </cell>
+          <cell r="D23">
+            <v>81.657855999999995</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>FC-1000</v>
+          </cell>
+          <cell r="B24">
+            <v>0.91</v>
+          </cell>
+          <cell r="C24">
+            <v>30.750720000000001</v>
+          </cell>
+          <cell r="D24">
+            <v>83.492863999999997</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1204,12 +1424,12 @@
       <c r="O4" s="1">
         <v>32</v>
       </c>
-      <c r="Q4" s="34" t="s">
+      <c r="Q4" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="35"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="37"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="38"/>
       <c r="U4" s="3"/>
     </row>
     <row r="5" spans="4:25" ht="30">
@@ -2407,10 +2627,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:AJ42"/>
+  <dimension ref="D4:AM42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z37" sqref="Z37"/>
+    <sheetView tabSelected="1" topLeftCell="E20" workbookViewId="0">
+      <selection activeCell="AF30" sqref="AF30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2422,26 +2642,29 @@
     <col min="20" max="20" width="14.6640625" style="1" customWidth="1"/>
     <col min="21" max="23" width="10.83203125" style="1"/>
     <col min="24" max="24" width="11.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="10.83203125" style="1"/>
-    <col min="27" max="27" width="11.83203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.83203125" style="1"/>
-    <col min="29" max="29" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="70.6640625" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="1"/>
+    <col min="25" max="25" width="10.83203125" style="1"/>
+    <col min="26" max="26" width="10.83203125" style="33"/>
+    <col min="27" max="28" width="10.83203125" style="1"/>
+    <col min="29" max="29" width="11.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.83203125" style="1"/>
+    <col min="31" max="31" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.83203125" style="22" customWidth="1"/>
+    <col min="33" max="33" width="70.6640625" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:36">
-      <c r="M4" s="38" t="s">
+    <row r="4" spans="4:39">
+      <c r="M4" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="41"/>
       <c r="P4" s="3"/>
       <c r="V4" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="4:36" ht="30">
+    <row r="5" spans="4:39" ht="30">
       <c r="E5" s="12" t="s">
         <v>0</v>
       </c>
@@ -2499,23 +2722,29 @@
       <c r="Y5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="Z5" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AA5" s="28" t="s">
+      <c r="AB5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC5" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AD5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AD5" s="31" t="s">
+      <c r="AG5" s="31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="4:36">
+    <row r="6" spans="4:39">
       <c r="D6" s="8" t="s">
         <v>3</v>
       </c>
@@ -2540,7 +2769,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="9"/>
     </row>
-    <row r="7" spans="4:36">
+    <row r="7" spans="4:39">
       <c r="D7" s="9"/>
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
@@ -2554,7 +2783,7 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="9"/>
     </row>
-    <row r="8" spans="4:36">
+    <row r="8" spans="4:39">
       <c r="D8" s="9" t="s">
         <v>13</v>
       </c>
@@ -2625,23 +2854,35 @@
         <f>E8*F8*G8/32</f>
         <v>9075</v>
       </c>
-      <c r="Z8" s="1">
+      <c r="Z8" s="33">
+        <f>Y8/$Y$27</f>
+        <v>0.44046983449012278</v>
+      </c>
+      <c r="AA8" s="1">
         <f>I8*J8*G6</f>
         <v>363</v>
       </c>
-      <c r="AA8" s="28">
+      <c r="AB8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC8" s="28">
         <f>Y8/$Y$27</f>
         <v>0.44046983449012278</v>
       </c>
-      <c r="AB8" s="1">
-        <v>25</v>
-      </c>
-      <c r="AC8" s="33">
+      <c r="AD8" s="1">
+        <f>VLOOKUP(AB8,[1]Summary!$A$16:$D$24,3,FALSE)</f>
+        <v>24.66816</v>
+      </c>
+      <c r="AE8" s="33">
         <f>L8/$L$28</f>
         <v>0.37590091955927429</v>
       </c>
-    </row>
-    <row r="9" spans="4:36">
+      <c r="AF8" s="22">
+        <f>AD8*Z8</f>
+        <v>10.865580352375867</v>
+      </c>
+    </row>
+    <row r="9" spans="4:39">
       <c r="D9" s="9"/>
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
@@ -2658,7 +2899,7 @@
       <c r="S9" s="15"/>
       <c r="T9" s="15"/>
     </row>
-    <row r="10" spans="4:36">
+    <row r="10" spans="4:39">
       <c r="D10" s="9" t="s">
         <v>11</v>
       </c>
@@ -2717,12 +2958,36 @@
       <c r="W10" s="1">
         <v>4</v>
       </c>
-      <c r="Z10" s="1">
+      <c r="X10" s="15">
+        <f>L10*W10</f>
+        <v>279936</v>
+      </c>
+      <c r="Y10" s="1">
+        <f>E10*F10*G10/32</f>
+        <v>2187</v>
+      </c>
+      <c r="AA10" s="1">
         <f>I10*J10*G8</f>
         <v>384</v>
       </c>
-    </row>
-    <row r="11" spans="4:36">
+      <c r="AB10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC10" s="28">
+        <f>Y10/$Y$27</f>
+        <v>0.10614958986555356</v>
+      </c>
+      <c r="AD10" s="1">
+        <f>VLOOKUP(AB10,[1]Summary!$A$16:$D$24,3,FALSE)</f>
+        <v>24.66816</v>
+      </c>
+      <c r="AE10" s="33"/>
+      <c r="AF10" s="22">
+        <f>AD10*AE10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="4:39">
       <c r="D11" s="9"/>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
@@ -2739,7 +3004,7 @@
       <c r="S11" s="15"/>
       <c r="T11" s="15"/>
     </row>
-    <row r="12" spans="4:36">
+    <row r="12" spans="4:39">
       <c r="D12" s="9" t="s">
         <v>13</v>
       </c>
@@ -2810,26 +3075,38 @@
         <f>E12*F12*G12/32</f>
         <v>5832</v>
       </c>
-      <c r="Z12" s="1">
+      <c r="Z12" s="33">
+        <f>Y12/$Y$27</f>
+        <v>0.2830655729748095</v>
+      </c>
+      <c r="AA12" s="1">
         <f>I12*J12*G10</f>
         <v>2400</v>
       </c>
-      <c r="AA12" s="28">
+      <c r="AB12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC12" s="28">
         <f>Y12/$Y$27</f>
         <v>0.2830655729748095</v>
       </c>
-      <c r="AB12" s="1">
-        <v>30</v>
-      </c>
-      <c r="AC12" s="33">
+      <c r="AD12" s="1">
+        <f>VLOOKUP(AB12,[1]Summary!$A$16:$D$24,3,FALSE)</f>
+        <v>30.07488</v>
+      </c>
+      <c r="AE12" s="33">
         <f>L12/$L$28</f>
         <v>0.24157070665230718</v>
       </c>
-      <c r="AJ12" s="1">
+      <c r="AF12" s="22">
+        <f>AD12*Z12</f>
+        <v>8.513163139348638</v>
+      </c>
+      <c r="AM12" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="4:36">
+    <row r="13" spans="4:39">
       <c r="D13" s="9"/>
       <c r="E13" s="2"/>
       <c r="F13" s="3"/>
@@ -2846,7 +3123,7 @@
       <c r="S13" s="15"/>
       <c r="T13" s="15"/>
     </row>
-    <row r="14" spans="4:36">
+    <row r="14" spans="4:39">
       <c r="D14" s="9" t="s">
         <v>14</v>
       </c>
@@ -2905,12 +3182,35 @@
       <c r="W14" s="1">
         <v>4</v>
       </c>
-      <c r="Z14" s="1">
+      <c r="X14" s="15">
+        <f>L14*W14</f>
+        <v>173056</v>
+      </c>
+      <c r="Y14" s="1">
+        <f>E14*F14*G14/32</f>
+        <v>1352</v>
+      </c>
+      <c r="AA14" s="1">
         <f>I14*J14*G12</f>
         <v>1024</v>
       </c>
-    </row>
-    <row r="15" spans="4:36">
+      <c r="AB14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC14" s="28">
+        <f>Y14/$Y$27</f>
+        <v>6.5621511430374216E-2</v>
+      </c>
+      <c r="AD14" s="1">
+        <f>VLOOKUP(AB14,[1]Summary!$A$16:$D$24,3,FALSE)</f>
+        <v>30.07488</v>
+      </c>
+      <c r="AE14" s="33">
+        <f>L14/$L$28</f>
+        <v>5.6001988236268743E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="4:39">
       <c r="D15" s="9"/>
       <c r="E15" s="2"/>
       <c r="F15" s="3"/>
@@ -2927,7 +3227,7 @@
       <c r="S15" s="15"/>
       <c r="T15" s="15"/>
     </row>
-    <row r="16" spans="4:36">
+    <row r="16" spans="4:39">
       <c r="D16" s="9" t="s">
         <v>13</v>
       </c>
@@ -2998,23 +3298,35 @@
         <f>E16*F16*G16/32</f>
         <v>2028</v>
       </c>
-      <c r="Z16" s="1">
+      <c r="Z16" s="33">
+        <f>Y16/$Y$27</f>
+        <v>9.8432267145561331E-2</v>
+      </c>
+      <c r="AA16" s="1">
         <f>I16*J16*G14</f>
         <v>2304</v>
       </c>
-      <c r="AA16" s="28">
+      <c r="AB16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC16" s="28">
         <f>Y16/$Y$27</f>
         <v>9.8432267145561331E-2</v>
       </c>
-      <c r="AB16" s="1">
-        <v>30</v>
-      </c>
-      <c r="AC16" s="33">
+      <c r="AD16" s="1">
+        <f>VLOOKUP(AB16,[1]Summary!$A$16:$D$24,3,FALSE)</f>
+        <v>30.07488</v>
+      </c>
+      <c r="AE16" s="33">
         <f>L16/$L$28</f>
         <v>8.4002982354403122E-2</v>
       </c>
-    </row>
-    <row r="17" spans="4:30">
+      <c r="AF16" s="22">
+        <f>AD16*Z16</f>
+        <v>2.9603386225306996</v>
+      </c>
+    </row>
+    <row r="17" spans="4:33">
       <c r="D17" s="9"/>
       <c r="E17" s="2"/>
       <c r="F17" s="3"/>
@@ -3031,7 +3343,7 @@
       <c r="S17" s="15"/>
       <c r="T17" s="15"/>
     </row>
-    <row r="18" spans="4:30">
+    <row r="18" spans="4:33">
       <c r="D18" s="9" t="s">
         <v>13</v>
       </c>
@@ -3102,23 +3414,35 @@
         <f>E18*F18*G18/32</f>
         <v>2028</v>
       </c>
-      <c r="Z18" s="1">
+      <c r="Z18" s="33">
+        <f>Y18/$Y$27</f>
+        <v>9.8432267145561331E-2</v>
+      </c>
+      <c r="AA18" s="1">
         <f>I18*J18*G16</f>
         <v>3456</v>
       </c>
-      <c r="AA18" s="28">
+      <c r="AB18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC18" s="28">
         <f>Y18/$Y$27</f>
         <v>9.8432267145561331E-2</v>
       </c>
-      <c r="AB18" s="1">
-        <v>30</v>
-      </c>
-      <c r="AC18" s="33">
+      <c r="AD18" s="1">
+        <f>VLOOKUP(AB18,[1]Summary!$A$16:$D$24,3,FALSE)</f>
+        <v>30.07488</v>
+      </c>
+      <c r="AE18" s="33">
         <f>L18/$L$28</f>
         <v>8.4002982354403122E-2</v>
       </c>
-    </row>
-    <row r="19" spans="4:30">
+      <c r="AF18" s="22">
+        <f>AD18*Z18</f>
+        <v>2.9603386225306996</v>
+      </c>
+    </row>
+    <row r="19" spans="4:33">
       <c r="D19" s="9"/>
       <c r="E19" s="2"/>
       <c r="F19" s="3"/>
@@ -3135,7 +3459,7 @@
       <c r="S19" s="15"/>
       <c r="T19" s="15"/>
     </row>
-    <row r="20" spans="4:30">
+    <row r="20" spans="4:33">
       <c r="D20" s="9" t="s">
         <v>13</v>
       </c>
@@ -3206,23 +3530,35 @@
         <f>E20*F20*G20/32</f>
         <v>1352</v>
       </c>
-      <c r="Z20" s="1">
+      <c r="Z20" s="33">
+        <f>Y20/$Y$27</f>
+        <v>6.5621511430374216E-2</v>
+      </c>
+      <c r="AA20" s="1">
         <f>I20*J20*G18</f>
         <v>3456</v>
       </c>
-      <c r="AA20" s="28">
+      <c r="AB20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC20" s="28">
         <f>Y20/$Y$27</f>
         <v>6.5621511430374216E-2</v>
       </c>
-      <c r="AB20" s="1">
-        <v>30</v>
-      </c>
-      <c r="AC20" s="33">
+      <c r="AD20" s="1">
+        <f>VLOOKUP(AB20,[1]Summary!$A$16:$D$24,3,FALSE)</f>
+        <v>30.07488</v>
+      </c>
+      <c r="AE20" s="33">
         <f>L20/$L$28</f>
         <v>5.6001988236268743E-2</v>
       </c>
-    </row>
-    <row r="21" spans="4:30">
+      <c r="AF20" s="22">
+        <f>AD20*Z20</f>
+        <v>1.9735590816871329</v>
+      </c>
+    </row>
+    <row r="21" spans="4:33">
       <c r="D21" s="9"/>
       <c r="E21" s="2"/>
       <c r="F21" s="3"/>
@@ -3239,7 +3575,7 @@
       <c r="S21" s="15"/>
       <c r="T21" s="15"/>
     </row>
-    <row r="22" spans="4:30">
+    <row r="22" spans="4:33">
       <c r="D22" s="9" t="s">
         <v>15</v>
       </c>
@@ -3306,23 +3642,35 @@
         <f>E22*F22*G22/32</f>
         <v>128</v>
       </c>
-      <c r="Z22" s="1">
+      <c r="Z22" s="33">
+        <f>Y22/$Y$27</f>
+        <v>6.2126874726981512E-3</v>
+      </c>
+      <c r="AA22" s="1">
         <f>I22*J22*G20</f>
         <v>43264</v>
       </c>
-      <c r="AA22" s="28">
+      <c r="AB22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC22" s="28">
         <f>Y22/$Y$27</f>
         <v>6.2126874726981512E-3</v>
       </c>
-      <c r="AB22" s="1">
-        <v>31</v>
-      </c>
-      <c r="AC22" s="33">
+      <c r="AD22" s="1">
+        <f>VLOOKUP(AB22,[1]Summary!$A$16:$D$24,3,FALSE)</f>
+        <v>31.764479999999999</v>
+      </c>
+      <c r="AE22" s="33">
         <f>L22/$L$28</f>
         <v>5.3019633833153836E-3</v>
       </c>
-    </row>
-    <row r="23" spans="4:30">
+      <c r="AF22" s="22">
+        <f>AD22*Z22</f>
+        <v>0.19734278697277097</v>
+      </c>
+    </row>
+    <row r="23" spans="4:33">
       <c r="D23" s="9"/>
       <c r="E23" s="2"/>
       <c r="F23" s="3"/>
@@ -3339,7 +3687,7 @@
       <c r="S23" s="15"/>
       <c r="T23" s="15"/>
     </row>
-    <row r="24" spans="4:30">
+    <row r="24" spans="4:33">
       <c r="D24" s="9" t="s">
         <v>15</v>
       </c>
@@ -3406,26 +3754,38 @@
         <f>E24*F24*G24/32</f>
         <v>128</v>
       </c>
-      <c r="Z24" s="1">
+      <c r="Z24" s="33">
+        <f>Y24/$Y$27</f>
+        <v>6.2126874726981512E-3</v>
+      </c>
+      <c r="AA24" s="1">
         <f>J24*G22</f>
         <v>4096</v>
       </c>
-      <c r="AA24" s="28">
+      <c r="AB24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC24" s="28">
         <f>Y24/$Y$27</f>
         <v>6.2126874726981512E-3</v>
       </c>
-      <c r="AB24" s="1">
-        <v>31</v>
-      </c>
-      <c r="AC24" s="33">
+      <c r="AD24" s="1">
+        <f>VLOOKUP(AB24,[1]Summary!$A$16:$D$24,3,FALSE)</f>
+        <v>31.764479999999999</v>
+      </c>
+      <c r="AE24" s="33">
         <f>L24/$L$28</f>
         <v>5.3019633833153836E-3</v>
       </c>
-      <c r="AD24" s="30" t="s">
+      <c r="AF24" s="22">
+        <f>AD24*Z24</f>
+        <v>0.19734278697277097</v>
+      </c>
+      <c r="AG24" s="30" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="4:30">
+    <row r="25" spans="4:33">
       <c r="D25" s="9"/>
       <c r="E25" s="2"/>
       <c r="F25" s="3"/>
@@ -3442,7 +3802,7 @@
       <c r="S25" s="15"/>
       <c r="T25" s="15"/>
     </row>
-    <row r="26" spans="4:30">
+    <row r="26" spans="4:33">
       <c r="D26" s="10" t="s">
         <v>15</v>
       </c>
@@ -3509,51 +3869,64 @@
         <f>E26*F26*G26/32</f>
         <v>32</v>
       </c>
-      <c r="Z26" s="1">
+      <c r="Z26" s="33">
+        <f>Y26/$Y$27</f>
+        <v>1.5531718681745378E-3</v>
+      </c>
+      <c r="AA26" s="1">
         <f>J26*G24</f>
         <v>4096</v>
       </c>
-      <c r="AA26" s="28">
+      <c r="AB26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC26" s="28">
         <f>Y26/$Y$27</f>
         <v>1.5531718681745378E-3</v>
       </c>
-      <c r="AB26" s="1">
-        <v>30</v>
-      </c>
-      <c r="AC26" s="33">
+      <c r="AD26" s="1">
+        <f>VLOOKUP(AB26,[1]Summary!$A$16:$D$24,3,FALSE)</f>
+        <v>31.764479999999999</v>
+      </c>
+      <c r="AE26" s="33">
         <f>L26/$L$28</f>
         <v>1.3254908458288459E-3</v>
       </c>
-      <c r="AD26" s="30" t="s">
+      <c r="AF26" s="22">
+        <f>AD26*Z26</f>
+        <v>4.9335696743192742E-2</v>
+      </c>
+      <c r="AG26" s="30" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="4:30">
+    <row r="27" spans="4:33">
       <c r="Q27" s="15"/>
       <c r="R27" s="15"/>
       <c r="S27" s="15"/>
       <c r="X27" s="15">
         <f>SUM(X8:X26)</f>
-        <v>1274815008</v>
+        <v>1275268000</v>
       </c>
       <c r="Y27" s="1">
-        <f>SUM(Y8:Y26)</f>
+        <f>Y8+Y12+Y16+Y18+Y20+Y22+Y24+Y26</f>
         <v>20603</v>
       </c>
-      <c r="AA27" s="1">
-        <f>SUM(AA8:AA26)</f>
-        <v>0.99999999999999978</v>
-      </c>
-      <c r="AB27" s="29">
-        <f>AVERAGE(AB8:AB26)</f>
-        <v>29.625</v>
-      </c>
-      <c r="AC27" s="29">
-        <f>AC8*Z8+AC12*Z12+AC16*Z16+AC18*Z18+AC20*Z20+AC22*Z22+AC24*Z24+AC26*Z26</f>
+      <c r="AC27" s="1">
+        <f>SUM(AC8:AC26)</f>
+        <v>1.1717711012959278</v>
+      </c>
+      <c r="AD27" s="29">
+        <f>AVERAGE(AD8:AD26)</f>
+        <v>29.500416000000001</v>
+      </c>
+      <c r="AE27" s="29">
+        <f>AE8*AA8+AE12*AA12+AE16*AA16+AE18*AA18+AE20*AA20+AE22*AA22+AE24*AA24+AE26*AA26</f>
         <v>1650.1519758097922</v>
       </c>
-    </row>
-    <row r="28" spans="4:30" ht="30">
+      <c r="AF27" s="34"/>
+    </row>
+    <row r="28" spans="4:33" ht="30">
       <c r="L28" s="1">
         <f>SUM(L8:L26)</f>
         <v>772544</v>
@@ -3573,14 +3946,18 @@
       </c>
       <c r="X28" s="15">
         <f>X27/SUM(L8:L26)</f>
-        <v>1650.151975809792</v>
+        <v>1650.7383398227155</v>
       </c>
       <c r="Y28" s="1">
         <f>Y27*32+L10+L14</f>
         <v>772544</v>
       </c>
-    </row>
-    <row r="29" spans="4:30">
+      <c r="Z28" s="33">
+        <f>SUM(Z8:Z26)</f>
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="29" spans="4:33">
       <c r="L29" s="1" t="s">
         <v>23</v>
       </c>
@@ -3595,26 +3972,39 @@
       <c r="Q29" s="15"/>
       <c r="R29" s="15"/>
     </row>
-    <row r="30" spans="4:30">
+    <row r="30" spans="4:33" ht="30">
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
       <c r="S30" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="4:30">
+      <c r="AE30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF30" s="22">
+        <f>SUM(AF8:AF26)</f>
+        <v>27.717001089161773</v>
+      </c>
+    </row>
+    <row r="31" spans="4:33">
       <c r="Q31" s="15"/>
       <c r="R31" s="15"/>
     </row>
-    <row r="32" spans="4:30">
+    <row r="32" spans="4:33">
       <c r="Q32" s="15"/>
       <c r="R32" s="15"/>
-    </row>
-    <row r="33" spans="15:18">
+      <c r="AA32" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="15:27">
       <c r="Q33" s="15"/>
       <c r="R33" s="15"/>
-    </row>
-    <row r="34" spans="15:18" ht="30">
+      <c r="AA33" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="15:27" ht="30">
       <c r="O34" s="12" t="s">
         <v>24</v>
       </c>
@@ -3625,11 +4015,11 @@
       </c>
       <c r="R34" s="15"/>
     </row>
-    <row r="35" spans="15:18">
+    <row r="35" spans="15:27">
       <c r="Q35" s="15"/>
       <c r="R35" s="15"/>
     </row>
-    <row r="36" spans="15:18">
+    <row r="36" spans="15:27">
       <c r="O36" s="1" t="s">
         <v>18</v>
       </c>
@@ -3639,7 +4029,7 @@
         <v>174157311424</v>
       </c>
     </row>
-    <row r="37" spans="15:18" ht="30">
+    <row r="37" spans="15:27" ht="30">
       <c r="O37" s="1" t="s">
         <v>19</v>
       </c>
@@ -3648,7 +4038,7 @@
       </c>
       <c r="Q37" s="15"/>
     </row>
-    <row r="38" spans="15:18" ht="30">
+    <row r="38" spans="15:27" ht="30">
       <c r="O38" s="1" t="s">
         <v>20</v>
       </c>
@@ -3658,7 +4048,7 @@
         <v>1393258491392</v>
       </c>
     </row>
-    <row r="39" spans="15:18" ht="30">
+    <row r="39" spans="15:27" ht="30">
       <c r="O39" s="1" t="s">
         <v>25</v>
       </c>
@@ -3667,7 +4057,7 @@
       </c>
       <c r="Q39" s="15"/>
     </row>
-    <row r="40" spans="15:18">
+    <row r="40" spans="15:27">
       <c r="O40" s="1" t="s">
         <v>21</v>
       </c>
@@ -3677,7 +4067,7 @@
         <v>4458427172454400</v>
       </c>
     </row>
-    <row r="42" spans="15:18">
+    <row r="42" spans="15:27">
       <c r="O42" s="1" t="s">
         <v>10</v>
       </c>
@@ -3717,11 +4107,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="4:19">
-      <c r="M4" s="38" t="s">
+      <c r="M4" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="41"/>
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="4:19" ht="30">

</xml_diff>